<commit_message>
Added 1.1.0 of term
</commit_message>
<xml_diff>
--- a/term/CodeSystem-KLCommonproprietary.xlsx
+++ b/term/CodeSystem-KLCommonproprietary.xlsx
@@ -29,7 +29,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0</t>
+    <t>1.1.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -59,7 +59,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-06-07T11:52:14+02:00</t>
+    <t>2023-07-10T23:08:03+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -235,10 +235,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true" applyFont="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>

</xml_diff>